<commit_message>
working on image selection and security
</commit_message>
<xml_diff>
--- a/src/question_form_sample.xlsx
+++ b/src/question_form_sample.xlsx
@@ -1,27 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22730"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\www\eVoucherServer\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC0BC850-9D3C-4734-93FD-8A59AA56229B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED24DDC7-523B-4824-8858-9EE27EA3BB8A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5850" yWindow="1560" windowWidth="17325" windowHeight="11910" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9165" yWindow="1215" windowWidth="18540" windowHeight="12345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
     <sheet name="工作表1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029" forceFullCalc="1"/>
+  <calcPr calcId="191029" forceFullCalc="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -29,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="63">
   <si>
     <t>type</t>
   </si>
@@ -216,17 +218,33 @@
   </si>
   <si>
     <t>system-page</t>
+  </si>
+  <si>
+    <t>Address Line 2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="細明體"/>
+      <family val="3"/>
+      <charset val="136"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -249,11 +267,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
@@ -561,7 +580,7 @@
   <dimension ref="A1:Q17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:XFD17"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -705,8 +724,8 @@
       <c r="A8" t="s">
         <v>23</v>
       </c>
-      <c r="B8" t="s">
-        <v>24</v>
+      <c r="B8" s="2" t="s">
+        <v>62</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -879,7 +898,9 @@
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1133,7 +1154,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="240" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" ht="210" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>28</v>
       </c>
@@ -1189,6 +1210,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>